<commit_message>
- reverted back some changes for IPP
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\GitProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergiu.wittenberger\Documents\UiPath\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F367E9-3F4B-45A4-8445-8FEA905F7D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69C3418-E688-40DA-9F9F-D8890EC413BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
-    <sheet name="InvoicePostProcessing" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="150">
   <si>
     <t>Name</t>
   </si>
@@ -484,121 +483,13 @@
   </si>
   <si>
     <t>https://ai-uipath.deskover.com/public/mlskills/34f238ca-8576-423d-a31b-3cc9cdc54a1f/930aa3d7-b4f8-4acd-8347-37fa1bc919a8/hachinvoices</t>
-  </si>
-  <si>
-    <t>ConfidenceFields</t>
-  </si>
-  <si>
-    <t>SubTotalAdditions</t>
-  </si>
-  <si>
-    <t>tax, shipping-handling, discount, tariff</t>
-  </si>
-  <si>
-    <t>MandatoryFields</t>
-  </si>
-  <si>
-    <t>date,invoice-number,po-no,total</t>
-  </si>
-  <si>
-    <t>MandatoryColumnFields</t>
-  </si>
-  <si>
-    <t>quantity,unit-price,line-amount</t>
-  </si>
-  <si>
-    <t>tax,net-amount,discount,shipping-handling,billing-name,total,tariff</t>
-  </si>
-  <si>
-    <t>date,shipping-address,invoice-number,po-no</t>
-  </si>
-  <si>
-    <t>Each field present in the list here, will be added to the subtotal to compute the total</t>
-  </si>
-  <si>
-    <t>These fields are mandatory. If they have not been extracted at all, the document will be sent for validation</t>
-  </si>
-  <si>
-    <t>These column fields are mandatory. If they have not been extracted at all, the document will be sent for validation</t>
-  </si>
-  <si>
-    <t>List of fields which will be checked versus a specific confidence threshold. All new entries must have the "-Confidence" suffix</t>
-  </si>
-  <si>
-    <t>List of fields which will be checked versus a single confidence #:  Other-Confidence</t>
-  </si>
-  <si>
-    <t>OtherConfidenceFields</t>
-  </si>
-  <si>
-    <t>date-Confidence</t>
-  </si>
-  <si>
-    <t>shipping-address-Confidence</t>
-  </si>
-  <si>
-    <t>invoice-number-Confidence</t>
-  </si>
-  <si>
-    <t>po-no-Confidence</t>
-  </si>
-  <si>
-    <t>other-Confidence</t>
-  </si>
-  <si>
-    <t>LogMessage_InvoicePostProcessing</t>
-  </si>
-  <si>
-    <t>Starting Invoice Post Processing</t>
-  </si>
-  <si>
-    <t>Quantity * Unit-price is not equal to Line Amount!</t>
-  </si>
-  <si>
-    <t>LogMessage_InvoicePostProcessing_LineAmountFailure</t>
-  </si>
-  <si>
-    <t>LogMessage_InvoicePostProcessing_MandatoryFieldsFailure</t>
-  </si>
-  <si>
-    <t>One or more of the mandatory were missing!</t>
-  </si>
-  <si>
-    <t>LogMessage_InvoicePostProcessing_DateFailure</t>
-  </si>
-  <si>
-    <t>Parsing the Date has failed!</t>
-  </si>
-  <si>
-    <t>LogMessage_InvoicePostProcessing_AlreadySetFalse</t>
-  </si>
-  <si>
-    <t>AutoExtraction is already set to false in a previous step. Skipping rest of checks.</t>
-  </si>
-  <si>
-    <t>LogMessage_InvoicePostProcessing_SubtotalFailure</t>
-  </si>
-  <si>
-    <t>Subtotal computation failed!</t>
-  </si>
-  <si>
-    <t>LogMessage_InvoicePostProcessing_TotalFailure</t>
-  </si>
-  <si>
-    <t>Total Computation Failed</t>
-  </si>
-  <si>
-    <t>LogMessage_InvoicePostProcessing_ConfidenceFieldsFailure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These are the fields that failed: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -628,11 +519,6 @@
       <sz val="8"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -655,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -665,7 +551,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -983,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -2233,7 +2118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -4723,203 +4608,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251BD6D1-964A-430B-A986-F8A3092611A8}">
-  <dimension ref="A1:C22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="115" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>155</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15" t="s">
-        <v>158</v>
-      </c>
-      <c r="C15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B18" s="6">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B19" s="6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B20" s="6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B21" s="6">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B22" s="6">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Invoice Post Processing update for DU Template
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergiu.wittenberger\Documents\UiPath\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\GitProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354AE0B3-6B75-4EBC-9ECC-17992C7A205A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1B960B-8E07-4AC2-9451-A611D3BAD914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
+    <sheet name="InvoicePostProcessing" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="197">
   <si>
     <t>Name</t>
   </si>
@@ -483,13 +484,154 @@
   </si>
   <si>
     <t>https://du.uipath.com/ie/invoices</t>
+  </si>
+  <si>
+    <t>LogMessage_InvoicePostProcessing</t>
+  </si>
+  <si>
+    <t>Starting Invoice Post Processing</t>
+  </si>
+  <si>
+    <t>LogMessage_InvoicePostProcessing_DateFailure</t>
+  </si>
+  <si>
+    <t>Parsing the Date has failed!</t>
+  </si>
+  <si>
+    <t>LogMessage_InvoicePostProcessing_MandatoryFieldsFailure</t>
+  </si>
+  <si>
+    <t>One or more of the mandatory were missing!</t>
+  </si>
+  <si>
+    <t>LogMessage_InvoicePostProcessing_LineAmountFailureMath</t>
+  </si>
+  <si>
+    <t>Quantity * Unit-price is not equal to Line Amount!</t>
+  </si>
+  <si>
+    <t>LogMessage_InvoicePostProcessing_LineAmountFailureEmpty</t>
+  </si>
+  <si>
+    <t>Quantity or Unit-price is Empty!</t>
+  </si>
+  <si>
+    <t>LogMessage_InvoicePostProcessing_AlreadySetFalse</t>
+  </si>
+  <si>
+    <t>AutoExtraction is already set to false in a previous step. Skipping rest of checks.</t>
+  </si>
+  <si>
+    <t>LogMessage_InvoicePostProcessing_SubtotalFailure</t>
+  </si>
+  <si>
+    <t>Subtotal Failure with subtotal: {0} and net-amount {1}</t>
+  </si>
+  <si>
+    <t>LogMessage_InvoicePostProcessing_TotalFailure</t>
+  </si>
+  <si>
+    <t>Total Computation Failed!</t>
+  </si>
+  <si>
+    <t>LogMessage_InvoicePostProcessing_SubtotalPass</t>
+  </si>
+  <si>
+    <t>Subtotal Pass with subtotal: {0} and net-amount {1}</t>
+  </si>
+  <si>
+    <t>LogMessage_InvoicePostProcessing_ConfidenceFieldsFailure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These are the fields that failed: </t>
+  </si>
+  <si>
+    <t>SubTotalAdditions</t>
+  </si>
+  <si>
+    <t>Each field present in the list here, will be added to the subtotal to compute the total</t>
+  </si>
+  <si>
+    <t>MandatoryFields</t>
+  </si>
+  <si>
+    <t>These fields are mandatory. If they have not been extracted at all, the document will be sent for validation</t>
+  </si>
+  <si>
+    <t>MandatoryColumnFields</t>
+  </si>
+  <si>
+    <t>These column fields are mandatory. If they have not been extracted at all, the document will be sent for validation</t>
+  </si>
+  <si>
+    <t>ConfidenceFields</t>
+  </si>
+  <si>
+    <t>List of fields which will be checked versus a specific confidence threshold. All new entries must have the "-Confidence" suffix</t>
+  </si>
+  <si>
+    <t>OtherConfidenceFields</t>
+  </si>
+  <si>
+    <t>List of fields which will be checked versus a single confidence #:  Other-Confidence</t>
+  </si>
+  <si>
+    <t>other-Confidence</t>
+  </si>
+  <si>
+    <t>TestQueue</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>TestBucket</t>
+  </si>
+  <si>
+    <t>TestAction</t>
+  </si>
+  <si>
+    <t>AlwaysValidateExtractionWithActionCenter</t>
+  </si>
+  <si>
+    <t>Date,Invoice Number,PO Number,Total</t>
+  </si>
+  <si>
+    <t>Tax Amount,Shipping Charges,Discount</t>
+  </si>
+  <si>
+    <t>Date,Shipping Address,Invoice Number,PO Number</t>
+  </si>
+  <si>
+    <t>Quantity,Unit Price,Line Amount</t>
+  </si>
+  <si>
+    <t>Date-Confidence</t>
+  </si>
+  <si>
+    <t>Shipping Address-Confidence</t>
+  </si>
+  <si>
+    <t>Invoice Number-Confidence</t>
+  </si>
+  <si>
+    <t>PO Number-Confidence</t>
+  </si>
+  <si>
+    <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms, Currency,Discount</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>If set to true, validation will always go through validation station</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -518,6 +660,19 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -541,7 +696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -552,6 +707,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -869,15 +1028,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B10:B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+    <col min="3" max="3" width="135.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1004,6 +1163,9 @@
       <c r="A10" t="s">
         <v>38</v>
       </c>
+      <c r="B10" s="4" t="s">
+        <v>184</v>
+      </c>
       <c r="C10" s="5" t="s">
         <v>134</v>
       </c>
@@ -1012,6 +1174,9 @@
       <c r="A11" t="s">
         <v>39</v>
       </c>
+      <c r="B11" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="C11" s="5" t="s">
         <v>135</v>
       </c>
@@ -1020,6 +1185,9 @@
       <c r="A12" t="s">
         <v>40</v>
       </c>
+      <c r="B12" s="4" t="s">
+        <v>183</v>
+      </c>
       <c r="C12" t="s">
         <v>137</v>
       </c>
@@ -1036,6 +1204,9 @@
       <c r="A14" t="s">
         <v>87</v>
       </c>
+      <c r="B14" s="4" t="s">
+        <v>181</v>
+      </c>
       <c r="C14" t="s">
         <v>126</v>
       </c>
@@ -1043,6 +1214,9 @@
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>136</v>
@@ -1118,7 +1292,15 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
+      <c r="A25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1127,22 +1309,24 @@
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3549,13 +3733,12 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.140625" customWidth="1"/>
     <col min="4" max="27" width="65.42578125" customWidth="1"/>
   </cols>
@@ -3608,7 +3791,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+    </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4609,4 +4799,211 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="115" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B24">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B25">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit 1 Exception Message Arguments replaved with actual exceptions Improved Exception logging
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB720374-CA4B-427A-98CB-8804E8116AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC97B0F2-45E2-41A3-BB9A-C6679BBD3C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="30000" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,9 +222,6 @@
     <t>Data export started for:</t>
   </si>
   <si>
-    <t xml:space="preserve">Process was aborted due to: </t>
-  </si>
-  <si>
     <t>Presenting Classification Station</t>
   </si>
   <si>
@@ -408,9 +405,6 @@
     <t>Duration, in seconds, between re-execution attempts</t>
   </si>
   <si>
-    <t>Failed to process page range {0} in file {1}. Exception: {2}</t>
-  </si>
-  <si>
     <t>Action Catalog Name</t>
   </si>
   <si>
@@ -625,6 +619,12 @@
   </si>
   <si>
     <t>Classification finished</t>
+  </si>
+  <si>
+    <t>Process was aborted due to {0} with message: {1} Full Exception: {2}</t>
+  </si>
+  <si>
+    <t>Failed to process page range {0} in file {1} due to {2} with message: {3} Full Exception: {4}</t>
   </si>
 </sst>
 </file>
@@ -1104,13 +1104,13 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1118,7 +1118,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1126,24 +1126,24 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1170,38 +1170,38 @@
         <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1236,7 +1236,7 @@
         <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1244,55 +1244,55 @@
         <v>5</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
         <v>89</v>
       </c>
-      <c r="B21" t="s">
-        <v>90</v>
-      </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2295,8 +2295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2350,51 +2350,51 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B7" s="3">
         <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2405,7 +2405,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2447,15 +2447,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2468,15 +2468,15 @@
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
         <v>32</v>
@@ -2487,7 +2487,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2495,7 +2495,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2503,7 +2503,7 @@
         <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2511,7 +2511,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2524,10 +2524,10 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" t="s">
         <v>95</v>
-      </c>
-      <c r="B25" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2543,15 +2543,15 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2559,7 +2559,7 @@
         <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2567,7 +2567,7 @@
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2575,7 +2575,7 @@
         <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2583,7 +2583,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2612,119 +2612,119 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" t="s">
         <v>98</v>
-      </c>
-      <c r="B42" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>119</v>
+      </c>
+      <c r="B46" t="s">
         <v>120</v>
-      </c>
-      <c r="B46" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" t="s">
         <v>107</v>
-      </c>
-      <c r="B47" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" t="s">
         <v>109</v>
-      </c>
-      <c r="B48" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" t="s">
         <v>113</v>
-      </c>
-      <c r="B49" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" t="s">
         <v>103</v>
-      </c>
-      <c r="B53" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
         <v>105</v>
-      </c>
-      <c r="B54" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2733,7 +2733,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2758,7 +2758,7 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>195</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3793,18 +3793,18 @@
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4837,87 +4837,87 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -4925,62 +4925,62 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B22">
         <v>85</v>
@@ -4988,7 +4988,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B23">
         <v>80</v>
@@ -4996,7 +4996,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B24">
         <v>85</v>
@@ -5004,7 +5004,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B25">
         <v>85</v>
@@ -5012,7 +5012,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B26">
         <v>50</v>

</xml_diff>

<commit_message>
Added the Skip Classifier/Extractor Trainer logic Updated the SetTransactionProgress code to follow the same approach
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC97B0F2-45E2-41A3-BB9A-C6679BBD3C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB845361-A766-440A-90DF-3D88E3E16510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="30000" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="30000" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="206">
   <si>
     <t>Name</t>
   </si>
@@ -351,9 +351,6 @@
     <t>TransactionProgress_ExtractionValidation</t>
   </si>
   <si>
-    <t>Validating Data Extraction</t>
-  </si>
-  <si>
     <t>LogMessage_SetTransactionProgress</t>
   </si>
   <si>
@@ -573,18 +570,12 @@
     <t>True</t>
   </si>
   <si>
-    <t>AlwaysValidateExtraction </t>
-  </si>
-  <si>
     <t>DecimalRounding</t>
   </si>
   <si>
     <t>AlwaysValidateClassification</t>
   </si>
   <si>
-    <t>If set to true, validation will always go through manual validation</t>
-  </si>
-  <si>
     <t>LogMessage_ExtractionBusinessRuleValidationStart</t>
   </si>
   <si>
@@ -625,6 +616,42 @@
   </si>
   <si>
     <t>Failed to process page range {0} in file {1} due to {2} with message: {3} Full Exception: {4}</t>
+  </si>
+  <si>
+    <t>SkipClassifierTraining</t>
+  </si>
+  <si>
+    <t>SkipExtractorTraining</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>If set to True, classification will always go through manual validation. Asset value overwrites the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>If set to True, extracted data will always go through manual validation. Asset value overwrites the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>If set to True, classification will always go through manual validation. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>If set to True, extracted data will always go through manual validation. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>If set to True, classifier training will not be performed. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>If set to True, extractor training will not be performed. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>If set to True, classifier training will not be performed. Asset value overwrites the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>If set to True, extractor training will not be performed. Asset value overwrites the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Validating Extracted Data</t>
   </si>
 </sst>
 </file>
@@ -1028,15 +1055,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1008"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.88671875" customWidth="1"/>
     <col min="2" max="2" width="70.109375" customWidth="1"/>
-    <col min="3" max="3" width="135.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="131.77734375" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1104,13 +1131,13 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1153,7 +1180,7 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1162,7 +1189,7 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1170,18 +1197,18 @@
         <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1189,10 +1216,10 @@
         <v>78</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1201,7 +1228,7 @@
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1244,7 +1271,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
         <v>93</v>
@@ -1252,7 +1279,7 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B20" t="s">
         <v>87</v>
@@ -1278,25 +1305,45 @@
         <v>179</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2288,6 +2335,7 @@
     <hyperlink ref="B19" r:id="rId3" xr:uid="{25977FD7-D683-43E1-B69A-0E1CBCB81805}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2295,8 +2343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2388,13 +2436,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" s="3">
         <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2405,7 +2453,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2471,7 +2519,7 @@
         <v>76</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2487,7 +2535,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2495,7 +2543,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2511,7 +2559,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2551,7 +2599,7 @@
         <v>77</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2567,7 +2615,7 @@
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2583,7 +2631,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2612,35 +2660,35 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" t="s">
         <v>132</v>
-      </c>
-      <c r="B40" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2662,7 +2710,7 @@
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B44" t="s">
         <v>100</v>
@@ -2671,42 +2719,42 @@
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" t="s">
         <v>119</v>
-      </c>
-      <c r="B46" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" t="s">
         <v>106</v>
-      </c>
-      <c r="B47" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" t="s">
         <v>108</v>
-      </c>
-      <c r="B48" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" t="s">
         <v>112</v>
-      </c>
-      <c r="B49" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2724,7 +2772,7 @@
         <v>104</v>
       </c>
       <c r="B54" t="s">
-        <v>105</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2733,7 +2781,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2758,7 +2806,7 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3733,14 +3781,15 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.109375" customWidth="1"/>
-    <col min="4" max="27" width="65.44140625" customWidth="1"/>
+    <col min="4" max="4" width="106.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="27" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3793,22 +3842,48 @@
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>184</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4837,87 +4912,87 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" t="s">
         <v>136</v>
-      </c>
-      <c r="B3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
         <v>138</v>
-      </c>
-      <c r="B4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" t="s">
         <v>140</v>
-      </c>
-      <c r="B5" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" t="s">
         <v>142</v>
-      </c>
-      <c r="B6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" t="s">
         <v>144</v>
-      </c>
-      <c r="B7" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" t="s">
         <v>146</v>
-      </c>
-      <c r="B8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" t="s">
         <v>148</v>
-      </c>
-      <c r="B9" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" t="s">
         <v>150</v>
-      </c>
-      <c r="B10" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" t="s">
         <v>152</v>
-      </c>
-      <c r="B11" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" t="s">
         <v>154</v>
-      </c>
-      <c r="B13" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -4925,62 +5000,62 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" t="s">
         <v>156</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C16" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" t="s">
         <v>158</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C17" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" t="s">
         <v>160</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C18" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" t="s">
         <v>162</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C19" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" t="s">
         <v>164</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B22">
         <v>85</v>
@@ -4988,7 +5063,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B23">
         <v>80</v>
@@ -4996,7 +5071,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B24">
         <v>85</v>
@@ -5004,7 +5079,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B25">
         <v>85</v>
@@ -5012,7 +5087,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B26">
         <v>50</v>

</xml_diff>

<commit_message>
Update Log messages in both VB and C#
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C33BFE4-0375-40D1-AE4D-0F53C92287BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F3CE82-B48A-4B61-BE9A-9E6CBF1933D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="30000" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16848" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -591,12 +591,6 @@
     <t>Waiting on classification validation action #</t>
   </si>
   <si>
-    <t>Resuming after classification validation action #{0}. Document(s) classified as: {1}</t>
-  </si>
-  <si>
-    <t>Resuming after data validation action #{0}. Document: {1}</t>
-  </si>
-  <si>
     <t>Data extraction finished</t>
   </si>
   <si>
@@ -646,6 +640,12 @@
   </si>
   <si>
     <t>Auxiliary folder where the job will download files when resuming after a human-in-the-loop action. Only used if downloading the files is enabled</t>
+  </si>
+  <si>
+    <t>Resuming after data validation{0}. Document: {1}</t>
+  </si>
+  <si>
+    <t>Resuming after classification validation{0}. Document(s) classified as: {1}</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1129,7 +1129,7 @@
         <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1296,7 +1296,7 @@
         <v>174</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1307,29 +1307,29 @@
         <v>174</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>193</v>
-      </c>
       <c r="C25" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2331,8 +2331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2507,7 +2507,7 @@
         <v>76</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2547,7 +2547,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2587,7 +2587,7 @@
         <v>77</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2619,7 +2619,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2760,7 +2760,7 @@
         <v>104</v>
       </c>
       <c r="B54" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2769,7 +2769,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2794,7 +2794,7 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3836,7 +3836,7 @@
         <v>176</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3847,29 +3847,29 @@
         <v>181</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
DU Release 22.4.1 (#168)
* Updated to have net5 support

* Updated User Guide

* Correct compilation errors in InvoicePostProcessing workflow, remove the WIP tag

* Changes to make project compilable for net5. Use hard coded value for InvokeWorkflowFile Timeout

* Update Log messages in both VB and C#

* Update User Guide

* Remove C# support

* Update project.json

"requiresUserInteraction": true

Co-authored-by: alexandru-luca <alexandru-ionel.luca@uipath.com>
Co-authored-by: TeodoraPatrascu <teodora.patrascu@uipath.com>
Co-authored-by: alexandru-luca <48438754+alexandru-luca@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C33BFE4-0375-40D1-AE4D-0F53C92287BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F3CE82-B48A-4B61-BE9A-9E6CBF1933D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="30000" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16848" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -591,12 +591,6 @@
     <t>Waiting on classification validation action #</t>
   </si>
   <si>
-    <t>Resuming after classification validation action #{0}. Document(s) classified as: {1}</t>
-  </si>
-  <si>
-    <t>Resuming after data validation action #{0}. Document: {1}</t>
-  </si>
-  <si>
     <t>Data extraction finished</t>
   </si>
   <si>
@@ -646,6 +640,12 @@
   </si>
   <si>
     <t>Auxiliary folder where the job will download files when resuming after a human-in-the-loop action. Only used if downloading the files is enabled</t>
+  </si>
+  <si>
+    <t>Resuming after data validation{0}. Document: {1}</t>
+  </si>
+  <si>
+    <t>Resuming after classification validation{0}. Document(s) classified as: {1}</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1129,7 +1129,7 @@
         <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1296,7 +1296,7 @@
         <v>174</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1307,29 +1307,29 @@
         <v>174</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>193</v>
-      </c>
       <c r="C25" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2331,8 +2331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2507,7 +2507,7 @@
         <v>76</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2547,7 +2547,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2587,7 +2587,7 @@
         <v>77</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2619,7 +2619,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2760,7 +2760,7 @@
         <v>104</v>
       </c>
       <c r="B54" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2769,7 +2769,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2794,7 +2794,7 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3836,7 +3836,7 @@
         <v>176</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3847,29 +3847,29 @@
         <v>181</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated User Guide, updated project dependencies to the latest version.
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosmin.pandelache\PycharmProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt1\CSharp\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1187CD33-5A5C-4228-BD64-41A75B07630D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51A4105-8E6D-44D0-9A8E-30C6C0D3B572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="216">
   <si>
     <t>Name</t>
   </si>
@@ -381,9 +381,6 @@
     <t>ClassificationEndpoint</t>
   </si>
   <si>
-    <t>The name of the Orchestrator Queue</t>
-  </si>
-  <si>
     <t>Data\TempFolder</t>
   </si>
   <si>
@@ -402,21 +399,6 @@
     <t>Duration, in seconds, between re-execution attempts</t>
   </si>
   <si>
-    <t>Action Catalog Name</t>
-  </si>
-  <si>
-    <t>Path to the Orchestrator Folder where the Action Catalog resides</t>
-  </si>
-  <si>
-    <t>Path to the Orchestrator Folder where the Queue resides</t>
-  </si>
-  <si>
-    <t>Storage Bucket Name (required when Action Center is used)</t>
-  </si>
-  <si>
-    <t>Path inside  the Storage Bucket where actions will store the files</t>
-  </si>
-  <si>
     <t>MaxLockTimeout</t>
   </si>
   <si>
@@ -666,30 +648,47 @@
     <t>DU_QueuePath</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Notice</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> - Below settings will override assets value!</t>
-    </r>
+    <t>Action Catalog Name. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Action Catalog resides. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Storage Bucket Name (required when Action Center is used). The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Path inside  the Storage Bucket where actions will store the files. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>The name of the Orchestrator Queue. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Queue resides. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Action Catalog Name. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Action Catalog resides. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Storage Bucket Name (required when Action Center is used). Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Path inside  the Storage Bucket where actions will store the files. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>The name of the Orchestrator Queue. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Queue resides. Has a corresponding asset that can be configured to overwrite this setting.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -729,12 +728,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1090,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1168,13 +1161,13 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1250,7 +1243,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
         <v>93</v>
@@ -1279,112 +1272,108 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
-        <v>122</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5" t="s">
-        <v>123</v>
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>37</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="B25" s="4"/>
       <c r="C25" t="s">
-        <v>125</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" t="s">
-        <v>115</v>
+        <v>79</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="4"/>
-    </row>
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2358,7 +2347,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" xr:uid="{EF98B574-7169-43E5-821B-D4670F472688}"/>
@@ -2374,7 +2362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -2467,13 +2455,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B7" s="3">
         <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2484,7 +2472,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2550,7 +2538,7 @@
         <v>76</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2566,7 +2554,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2574,7 +2562,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2590,7 +2578,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2630,7 +2618,7 @@
         <v>77</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2646,7 +2634,7 @@
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2662,7 +2650,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2691,35 +2679,35 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2750,10 +2738,10 @@
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" t="s">
         <v>118</v>
-      </c>
-      <c r="B46" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2803,7 +2791,7 @@
         <v>104</v>
       </c>
       <c r="B54" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2812,7 +2800,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2837,7 +2825,7 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3811,8 +3799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3873,46 +3861,46 @@
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3925,10 +3913,10 @@
         <v>35</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>122</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3936,10 +3924,10 @@
         <v>36</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>123</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3947,21 +3935,21 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3969,10 +3957,10 @@
         <v>78</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" t="s">
         <v>208</v>
-      </c>
-      <c r="D12" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3980,10 +3968,10 @@
         <v>79</v>
       </c>
       <c r="B13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5008,87 +4996,87 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -5096,62 +5084,62 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C17" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C19" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B22">
         <v>85</v>
@@ -5159,7 +5147,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B23">
         <v>80</v>
@@ -5167,7 +5155,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B24">
         <v>85</v>
@@ -5175,7 +5163,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B25">
         <v>85</v>
@@ -5183,7 +5171,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B26">
         <v>50</v>

</xml_diff>

<commit_message>
Automatic detection of number of decimal points in InvoicePostProcessing.xaml
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\DU_Task\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F3CE82-B48A-4B61-BE9A-9E6CBF1933D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E4C0ED-36B0-49FF-89EB-CF4D725A82E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16848" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="203">
   <si>
     <t>Name</t>
   </si>
@@ -559,9 +559,6 @@
   </si>
   <si>
     <t>True</t>
-  </si>
-  <si>
-    <t>DecimalRounding</t>
   </si>
   <si>
     <t>AlwaysValidateClassification</t>
@@ -717,18 +714,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1049,7 +1043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1008"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1129,7 +1125,7 @@
         <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1170,8 +1166,8 @@
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1179,8 +1175,8 @@
       <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1188,7 +1184,7 @@
       <c r="A10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>125</v>
       </c>
@@ -1205,7 +1201,7 @@
       <c r="A12" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="3"/>
       <c r="C12" t="s">
         <v>115</v>
       </c>
@@ -1214,8 +1210,8 @@
       <c r="A13" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1258,7 +1254,7 @@
       <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="2" t="s">
         <v>133</v>
       </c>
       <c r="C19" t="s">
@@ -1289,47 +1285,47 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="C24" s="4" t="s">
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="B26" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1340,7 +1336,7 @@
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="4"/>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2331,7 +2327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -2393,7 +2389,7 @@
       <c r="A4" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
@@ -2404,7 +2400,7 @@
       <c r="A5" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
@@ -2415,7 +2411,7 @@
       <c r="A6" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
@@ -2426,10 +2422,10 @@
       <c r="A7" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>30</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2437,10 +2433,10 @@
       <c r="A8" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>30</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2490,7 +2486,7 @@
       <c r="A16" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2506,8 +2502,8 @@
       <c r="A18" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>186</v>
+      <c r="B18" s="3" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2523,7 +2519,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2531,7 +2527,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2547,7 +2543,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2583,11 +2579,11 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>185</v>
+      <c r="B28" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2603,7 +2599,7 @@
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2619,7 +2615,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2647,19 +2643,19 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B36" s="4" t="s">
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2760,7 +2756,7 @@
         <v>104</v>
       </c>
       <c r="B54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2769,7 +2765,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2794,11 +2790,11 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="6"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3829,47 +3825,47 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>192</v>
+      <c r="A3" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>193</v>
+        <v>180</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4874,10 +4870,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4888,13 +4884,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4980,104 +4976,96 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>175</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
+        <v>154</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>166</v>
+        <v>156</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="C16" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>156</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="C17" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>158</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>160</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="C19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C20" t="s">
         <v>163</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21">
+        <v>85</v>
+      </c>
+    </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>169</v>
+      <c r="A22" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="B22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B23">
-        <v>80</v>
-      </c>
-    </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>171</v>
+      <c r="A24" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="B24">
         <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>172</v>
+      <c r="A25" t="s">
+        <v>164</v>
       </c>
       <c r="B25">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>164</v>
-      </c>
-      <c r="B26">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add DU assets to config file. They were removed by mistake.
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\DU_Task\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\Unit_Module_Testing\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E4C0ED-36B0-49FF-89EB-CF4D725A82E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7638925C-5898-4667-940C-C81828151B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="215">
   <si>
     <t>Name</t>
   </si>
@@ -381,9 +381,6 @@
     <t>ClassificationEndpoint</t>
   </si>
   <si>
-    <t>The name of the Orchestrator Queue</t>
-  </si>
-  <si>
     <t>Data\TempFolder</t>
   </si>
   <si>
@@ -402,21 +399,6 @@
     <t>Duration, in seconds, between re-execution attempts</t>
   </si>
   <si>
-    <t>Action Catalog Name</t>
-  </si>
-  <si>
-    <t>Path to the Orchestrator Folder where the Action Catalog resides</t>
-  </si>
-  <si>
-    <t>Path to the Orchestrator Folder where the Queue resides</t>
-  </si>
-  <si>
-    <t>Storage Bucket Name (required when Action Center is used)</t>
-  </si>
-  <si>
-    <t>Path inside  the Storage Bucket where actions will store the files</t>
-  </si>
-  <si>
     <t>MaxLockTimeout</t>
   </si>
   <si>
@@ -643,6 +625,60 @@
   </si>
   <si>
     <t>Resuming after classification validation{0}. Document(s) classified as: {1}</t>
+  </si>
+  <si>
+    <t>DU_StorageBucketName</t>
+  </si>
+  <si>
+    <t>DU_StorageBucketDirectoryPath</t>
+  </si>
+  <si>
+    <t>DU_ActionFolderPath</t>
+  </si>
+  <si>
+    <t>DU_ActionCatalogName</t>
+  </si>
+  <si>
+    <t>DU_QueueName</t>
+  </si>
+  <si>
+    <t>DU_QueuePath</t>
+  </si>
+  <si>
+    <t>Action Catalog Name. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Action Catalog resides. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Storage Bucket Name (required when Action Center is used). The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Path inside  the Storage Bucket where actions will store the files. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>The name of the Orchestrator Queue. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Queue resides. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Action Catalog Name. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Action Catalog resides. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Storage Bucket Name (required when Action Center is used). Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Path inside  the Storage Bucket where actions will store the files. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>The name of the Orchestrator Queue. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Queue resides. Has a corresponding asset that can be configured to overwrite this setting.</t>
   </si>
 </sst>
 </file>
@@ -1041,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1008"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1119,13 +1155,13 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1164,194 +1200,193 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
       <c r="C8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" t="s">
-        <v>123</v>
-      </c>
-    </row>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C10" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
       <c r="C13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-    </row>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
+      <c r="A17" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" t="s">
-        <v>92</v>
+      <c r="A18" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" t="s">
-        <v>93</v>
+      <c r="A19" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="A20" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" t="s">
+        <v>209</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>193</v>
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>194</v>
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>195</v>
+      <c r="A25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="3"/>
+    </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2306,17 +2341,11 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" xr:uid="{EF98B574-7169-43E5-821B-D4670F472688}"/>
-    <hyperlink ref="B17" r:id="rId2" xr:uid="{A81C761C-FDC0-4FAC-9731-C4ED96819803}"/>
-    <hyperlink ref="B19" r:id="rId3" xr:uid="{25977FD7-D683-43E1-B69A-0E1CBCB81805}"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{EF98B574-7169-43E5-821B-D4670F472688}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{A81C761C-FDC0-4FAC-9731-C4ED96819803}"/>
+    <hyperlink ref="B12" r:id="rId3" xr:uid="{25977FD7-D683-43E1-B69A-0E1CBCB81805}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -2327,8 +2356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2420,13 +2449,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B7">
         <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2437,7 +2466,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2503,7 +2532,7 @@
         <v>76</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2519,7 +2548,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2527,7 +2556,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2543,7 +2572,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2583,7 +2612,7 @@
         <v>77</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2599,7 +2628,7 @@
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2615,7 +2644,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2644,35 +2673,35 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2703,10 +2732,10 @@
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" t="s">
         <v>118</v>
-      </c>
-      <c r="B46" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2756,7 +2785,7 @@
         <v>104</v>
       </c>
       <c r="B54" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2765,7 +2794,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2790,7 +2819,7 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3762,10 +3791,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3826,55 +3855,119 @@
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="D11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" t="s">
+        <v>208</v>
+      </c>
+    </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4862,6 +4955,7 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4872,8 +4966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4896,142 +4990,142 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C19" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B21">
         <v>85</v>
@@ -5039,7 +5133,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B22">
         <v>80</v>
@@ -5047,7 +5141,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B23">
         <v>85</v>
@@ -5055,7 +5149,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B24">
         <v>85</v>
@@ -5063,7 +5157,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B25">
         <v>50</v>

</xml_diff>

<commit_message>
Added first version of the test cases
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura.olaru\Desktop\GIT\DU\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5F082F-0DA4-488C-94A7-F14718A271FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312D80E7-E57F-4234-BD98-CD21B4ABC5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="212">
   <si>
     <t>Name</t>
   </si>
@@ -655,6 +655,21 @@
   </si>
   <si>
     <t>DU_ClassificationTreshold</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>LauraActionCatalog</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>LauraStorageBucket</t>
+  </si>
+  <si>
+    <t>DocumentUnderstandingQueue</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1071,7 @@
   <dimension ref="A1:Z1008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1193,9 @@
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="C8" t="s">
         <v>122</v>
       </c>
@@ -1187,7 +1204,9 @@
       <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="C9" t="s">
         <v>123</v>
       </c>
@@ -1196,7 +1215,9 @@
       <c r="A10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="C10" t="s">
         <v>125</v>
       </c>
@@ -1205,6 +1226,9 @@
       <c r="A11" t="s">
         <v>120</v>
       </c>
+      <c r="B11" t="s">
+        <v>209</v>
+      </c>
       <c r="C11" t="s">
         <v>126</v>
       </c>
@@ -1213,7 +1237,9 @@
       <c r="A12" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>211</v>
+      </c>
       <c r="C12" t="s">
         <v>115</v>
       </c>
@@ -1222,7 +1248,9 @@
       <c r="A13" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="C13" t="s">
         <v>124</v>
       </c>
@@ -3787,7 +3815,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3842,6 +3870,9 @@
       <c r="B2" t="s">
         <v>40</v>
       </c>
+      <c r="C2" t="s">
+        <v>207</v>
+      </c>
       <c r="D2" t="s">
         <v>38</v>
       </c>
@@ -3853,6 +3884,9 @@
       <c r="B3" s="3" t="s">
         <v>176</v>
       </c>
+      <c r="C3" t="s">
+        <v>207</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>192</v>
       </c>
@@ -3864,6 +3898,9 @@
       <c r="B4" t="s">
         <v>181</v>
       </c>
+      <c r="C4" t="s">
+        <v>207</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>193</v>
       </c>
@@ -3875,6 +3912,9 @@
       <c r="B5" s="3" t="s">
         <v>189</v>
       </c>
+      <c r="C5" t="s">
+        <v>207</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>198</v>
       </c>
@@ -3886,6 +3926,9 @@
       <c r="B6" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="C6" t="s">
+        <v>207</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>199</v>
       </c>
@@ -3896,6 +3939,9 @@
       </c>
       <c r="B7" s="3" t="s">
         <v>206</v>
+      </c>
+      <c r="C7" t="s">
+        <v>207</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>205</v>

</xml_diff>

<commit_message>
Added final modifications along with Config for test case
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura.olaru\Desktop\GIT\DU\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura.olaru\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312D80E7-E57F-4234-BD98-CD21B4ABC5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E91D854-0B79-4BED-BA8B-8721C59920D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="218">
   <si>
     <t>Name</t>
   </si>
@@ -381,9 +381,6 @@
     <t>ClassificationEndpoint</t>
   </si>
   <si>
-    <t>The name of the Orchestrator Queue</t>
-  </si>
-  <si>
     <t>Data\TempFolder</t>
   </si>
   <si>
@@ -402,21 +399,6 @@
     <t>Duration, in seconds, between re-execution attempts</t>
   </si>
   <si>
-    <t>Action Catalog Name</t>
-  </si>
-  <si>
-    <t>Path to the Orchestrator Folder where the Action Catalog resides</t>
-  </si>
-  <si>
-    <t>Path to the Orchestrator Folder where the Queue resides</t>
-  </si>
-  <si>
-    <t>Storage Bucket Name (required when Action Center is used)</t>
-  </si>
-  <si>
-    <t>Path inside  the Storage Bucket where actions will store the files</t>
-  </si>
-  <si>
     <t>MaxLockTimeout</t>
   </si>
   <si>
@@ -561,9 +543,6 @@
     <t>True</t>
   </si>
   <si>
-    <t>DecimalRounding</t>
-  </si>
-  <si>
     <t>AlwaysValidateClassification</t>
   </si>
   <si>
@@ -648,28 +627,67 @@
     <t>Resuming after classification validation{0}. Document(s) classified as: {1}</t>
   </si>
   <si>
+    <t>DU_StorageBucketName</t>
+  </si>
+  <si>
+    <t>DU_StorageBucketDirectoryPath</t>
+  </si>
+  <si>
+    <t>DU_ActionFolderPath</t>
+  </si>
+  <si>
+    <t>DU_ActionCatalogName</t>
+  </si>
+  <si>
+    <t>DU_QueueName</t>
+  </si>
+  <si>
+    <t>DU_QueuePath</t>
+  </si>
+  <si>
+    <t>Action Catalog Name. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Action Catalog resides. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Storage Bucket Name (required when Action Center is used). The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Path inside  the Storage Bucket where actions will store the files. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>The name of the Orchestrator Queue. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Queue resides. The asset value overrides the one from the "Settings" sheet</t>
+  </si>
+  <si>
+    <t>Action Catalog Name. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Action Catalog resides. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Storage Bucket Name (required when Action Center is used). Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Path inside  the Storage Bucket where actions will store the files. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>The name of the Orchestrator Queue. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Path to the Orchestrator Folder where the Queue resides. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
     <t>ClassificationThreshold</t>
   </si>
   <si>
+    <t>DU_ClassificationTreshold</t>
+  </si>
+  <si>
     <t>Classification treshold for Classification Business Rule Validation</t>
-  </si>
-  <si>
-    <t>DU_ClassificationTreshold</t>
-  </si>
-  <si>
-    <t>Shared</t>
-  </si>
-  <si>
-    <t>LauraActionCatalog</t>
-  </si>
-  <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>LauraStorageBucket</t>
-  </si>
-  <si>
-    <t>DocumentUnderstandingQueue</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1008"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1146,13 +1164,13 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1191,217 +1209,207 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>208</v>
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C9" t="s">
-        <v>123</v>
-      </c>
-    </row>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>210</v>
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" t="s">
-        <v>209</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>211</v>
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>209</v>
+        <v>114</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-    </row>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
+      <c r="A17" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" t="s">
-        <v>92</v>
+      <c r="A18" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" t="s">
-        <v>93</v>
+      <c r="A19" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" t="s">
-        <v>90</v>
+      <c r="A20" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
+      <c r="A21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>215</v>
+      </c>
+      <c r="B22">
+        <v>50</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>195</v>
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>196</v>
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>197</v>
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>204</v>
-      </c>
-      <c r="B27">
-        <v>50</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>119</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+    </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2358,15 +2366,11 @@
     <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" xr:uid="{EF98B574-7169-43E5-821B-D4670F472688}"/>
-    <hyperlink ref="B17" r:id="rId2" xr:uid="{A81C761C-FDC0-4FAC-9731-C4ED96819803}"/>
-    <hyperlink ref="B19" r:id="rId3" xr:uid="{25977FD7-D683-43E1-B69A-0E1CBCB81805}"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{EF98B574-7169-43E5-821B-D4670F472688}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{A81C761C-FDC0-4FAC-9731-C4ED96819803}"/>
+    <hyperlink ref="B12" r:id="rId3" xr:uid="{25977FD7-D683-43E1-B69A-0E1CBCB81805}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -2378,7 +2382,7 @@
   <dimension ref="A1:Z1018"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2470,13 +2474,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B7">
         <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2487,7 +2491,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2553,7 +2557,7 @@
         <v>76</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2569,7 +2573,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2577,7 +2581,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2593,7 +2597,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2633,7 +2637,7 @@
         <v>77</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2649,7 +2653,7 @@
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2665,7 +2669,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2694,35 +2698,35 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2753,10 +2757,10 @@
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" t="s">
         <v>118</v>
-      </c>
-      <c r="B46" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2806,7 +2810,7 @@
         <v>104</v>
       </c>
       <c r="B54" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2815,7 +2819,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2840,7 +2844,7 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3812,10 +3816,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3870,90 +3874,136 @@
       <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
-        <v>207</v>
-      </c>
       <c r="D2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C3" t="s">
-        <v>207</v>
+        <v>169</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
-      </c>
-      <c r="C4" t="s">
-        <v>207</v>
+        <v>174</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C5" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" t="s">
         <v>207</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C7" t="s">
-        <v>207</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4940,6 +4990,7 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4948,10 +4999,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4974,184 +5025,176 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>175</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
+        <v>148</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>163</v>
+      </c>
+      <c r="B21">
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B22">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B23">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B24">
         <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>172</v>
+      <c r="A25" t="s">
+        <v>158</v>
       </c>
       <c r="B25">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>164</v>
-      </c>
-      <c r="B26">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made changes and added more test data variations
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura.olaru\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura.olaru\Desktop\GIT\DU\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E91D854-0B79-4BED-BA8B-8721C59920D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D55435B-2134-4B61-8324-6F7420D14DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -688,6 +688,21 @@
   </si>
   <si>
     <t>Classification treshold for Classification Business Rule Validation</t>
+  </si>
+  <si>
+    <t>LauraActionCatalog</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>LauraStorageBucket</t>
+  </si>
+  <si>
+    <t>DocumentUnderstandingQueue</t>
+  </si>
+  <si>
+    <t>Shared</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1104,7 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1356,9 @@
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="C24" t="s">
         <v>209</v>
       </c>
@@ -1350,7 +1367,9 @@
       <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>219</v>
+      </c>
       <c r="C25" t="s">
         <v>210</v>
       </c>
@@ -1359,6 +1378,9 @@
       <c r="A26" t="s">
         <v>37</v>
       </c>
+      <c r="B26" t="s">
+        <v>220</v>
+      </c>
       <c r="C26" t="s">
         <v>211</v>
       </c>
@@ -1367,7 +1389,9 @@
       <c r="A27" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>219</v>
+      </c>
       <c r="C27" t="s">
         <v>212</v>
       </c>
@@ -1376,7 +1400,9 @@
       <c r="A28" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="C28" t="s">
         <v>213</v>
       </c>
@@ -1384,6 +1410,9 @@
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>79</v>
+      </c>
+      <c r="B29" t="s">
+        <v>219</v>
       </c>
       <c r="C29" t="s">
         <v>214</v>
@@ -3819,7 +3848,7 @@
   <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3874,6 +3903,9 @@
       <c r="B2" t="s">
         <v>40</v>
       </c>
+      <c r="C2" t="s">
+        <v>222</v>
+      </c>
       <c r="D2" t="s">
         <v>38</v>
       </c>
@@ -3885,6 +3917,9 @@
       <c r="B3" s="3" t="s">
         <v>169</v>
       </c>
+      <c r="C3" t="s">
+        <v>222</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>185</v>
       </c>
@@ -3896,6 +3931,9 @@
       <c r="B4" t="s">
         <v>174</v>
       </c>
+      <c r="C4" t="s">
+        <v>222</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>186</v>
       </c>
@@ -3907,6 +3945,9 @@
       <c r="B5" s="3" t="s">
         <v>182</v>
       </c>
+      <c r="C5" t="s">
+        <v>222</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>191</v>
       </c>
@@ -3917,6 +3958,9 @@
       </c>
       <c r="B6" s="3" t="s">
         <v>183</v>
+      </c>
+      <c r="C6" t="s">
+        <v>222</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>192</v>
@@ -3934,6 +3978,9 @@
       <c r="B8" s="3" t="s">
         <v>200</v>
       </c>
+      <c r="C8" t="s">
+        <v>222</v>
+      </c>
       <c r="D8" t="s">
         <v>203</v>
       </c>
@@ -3945,6 +3992,9 @@
       <c r="B9" s="3" t="s">
         <v>199</v>
       </c>
+      <c r="C9" t="s">
+        <v>222</v>
+      </c>
       <c r="D9" t="s">
         <v>204</v>
       </c>
@@ -3956,6 +4006,9 @@
       <c r="B10" t="s">
         <v>197</v>
       </c>
+      <c r="C10" t="s">
+        <v>222</v>
+      </c>
       <c r="D10" t="s">
         <v>205</v>
       </c>
@@ -3967,6 +4020,9 @@
       <c r="B11" s="3" t="s">
         <v>198</v>
       </c>
+      <c r="C11" t="s">
+        <v>222</v>
+      </c>
       <c r="D11" t="s">
         <v>206</v>
       </c>
@@ -3978,6 +4034,9 @@
       <c r="B12" s="3" t="s">
         <v>201</v>
       </c>
+      <c r="C12" t="s">
+        <v>222</v>
+      </c>
       <c r="D12" t="s">
         <v>207</v>
       </c>
@@ -3989,6 +4048,9 @@
       <c r="B13" t="s">
         <v>202</v>
       </c>
+      <c r="C13" t="s">
+        <v>222</v>
+      </c>
       <c r="D13" t="s">
         <v>208</v>
       </c>
@@ -3999,6 +4061,9 @@
       </c>
       <c r="B14" s="3" t="s">
         <v>216</v>
+      </c>
+      <c r="C14" t="s">
+        <v>222</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>217</v>

</xml_diff>

<commit_message>
Added BrValidationTestCase and yaml
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura.olaru\Desktop\GIT\DU\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5C3253-BFEE-41DF-AD21-FD5DFBFBE937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B206BB2-B0FE-45C5-A422-CF1DD389F8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="222">
   <si>
     <t>Name</t>
   </si>
@@ -684,10 +684,22 @@
     <t>ClassificationThreshold</t>
   </si>
   <si>
-    <t>DU_ClassificationTreshold</t>
-  </si>
-  <si>
-    <t>Classification treshold for Classification Business Rule Validation</t>
+    <t>DUActionCatalog</t>
+  </si>
+  <si>
+    <t>DU Insights</t>
+  </si>
+  <si>
+    <t>DUStorageBucket</t>
+  </si>
+  <si>
+    <t>DUQueue</t>
+  </si>
+  <si>
+    <t>Classification threshold for Classification Business Rule Validation must be a value between 0 and 1.</t>
+  </si>
+  <si>
+    <t>DU_ClassificationThreshold</t>
   </si>
 </sst>
 </file>
@@ -1088,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1281,7 +1293,7 @@
         <v>169</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>187</v>
@@ -1330,10 +1342,10 @@
         <v>215</v>
       </c>
       <c r="B22">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1353,9 @@
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>216</v>
+      </c>
       <c r="C24" t="s">
         <v>209</v>
       </c>
@@ -1350,7 +1364,9 @@
       <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" t="s">
+        <v>217</v>
+      </c>
       <c r="C25" t="s">
         <v>210</v>
       </c>
@@ -1359,6 +1375,9 @@
       <c r="A26" t="s">
         <v>37</v>
       </c>
+      <c r="B26" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="C26" t="s">
         <v>211</v>
       </c>
@@ -1367,7 +1386,9 @@
       <c r="A27" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" t="s">
+        <v>217</v>
+      </c>
       <c r="C27" t="s">
         <v>212</v>
       </c>
@@ -1376,7 +1397,9 @@
       <c r="A28" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="3" t="s">
+        <v>219</v>
+      </c>
       <c r="C28" t="s">
         <v>213</v>
       </c>
@@ -1384,6 +1407,9 @@
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>79</v>
+      </c>
+      <c r="B29" t="s">
+        <v>217</v>
       </c>
       <c r="C29" t="s">
         <v>214</v>
@@ -3818,8 +3844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3874,6 +3900,9 @@
       <c r="B2" t="s">
         <v>40</v>
       </c>
+      <c r="C2" t="s">
+        <v>217</v>
+      </c>
       <c r="D2" t="s">
         <v>38</v>
       </c>
@@ -3885,6 +3914,9 @@
       <c r="B3" s="3" t="s">
         <v>169</v>
       </c>
+      <c r="C3" t="s">
+        <v>217</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>185</v>
       </c>
@@ -3896,6 +3928,9 @@
       <c r="B4" t="s">
         <v>174</v>
       </c>
+      <c r="C4" t="s">
+        <v>217</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>186</v>
       </c>
@@ -3907,6 +3942,9 @@
       <c r="B5" s="3" t="s">
         <v>182</v>
       </c>
+      <c r="C5" t="s">
+        <v>217</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>191</v>
       </c>
@@ -3917,6 +3955,9 @@
       </c>
       <c r="B6" s="3" t="s">
         <v>183</v>
+      </c>
+      <c r="C6" t="s">
+        <v>217</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>192</v>
@@ -3934,6 +3975,9 @@
       <c r="B8" s="3" t="s">
         <v>200</v>
       </c>
+      <c r="C8" t="s">
+        <v>217</v>
+      </c>
       <c r="D8" t="s">
         <v>203</v>
       </c>
@@ -3945,6 +3989,9 @@
       <c r="B9" s="3" t="s">
         <v>199</v>
       </c>
+      <c r="C9" t="s">
+        <v>217</v>
+      </c>
       <c r="D9" t="s">
         <v>204</v>
       </c>
@@ -3956,6 +4003,9 @@
       <c r="B10" t="s">
         <v>197</v>
       </c>
+      <c r="C10" t="s">
+        <v>217</v>
+      </c>
       <c r="D10" t="s">
         <v>205</v>
       </c>
@@ -3967,6 +4017,9 @@
       <c r="B11" s="3" t="s">
         <v>198</v>
       </c>
+      <c r="C11" t="s">
+        <v>217</v>
+      </c>
       <c r="D11" t="s">
         <v>206</v>
       </c>
@@ -3978,6 +4031,9 @@
       <c r="B12" s="3" t="s">
         <v>201</v>
       </c>
+      <c r="C12" t="s">
+        <v>217</v>
+      </c>
       <c r="D12" t="s">
         <v>207</v>
       </c>
@@ -3989,6 +4045,9 @@
       <c r="B13" t="s">
         <v>202</v>
       </c>
+      <c r="C13" t="s">
+        <v>217</v>
+      </c>
       <c r="D13" t="s">
         <v>208</v>
       </c>
@@ -3998,10 +4057,13 @@
         <v>215</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>216</v>
+        <v>221</v>
+      </c>
+      <c r="C14" t="s">
+        <v>217</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Final modifications on VB and C#
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura.olaru\Desktop\GIT\DU\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B206BB2-B0FE-45C5-A422-CF1DD389F8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB760162-D958-4309-8A46-E82C7FAB0BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="218">
   <si>
     <t>Name</t>
   </si>
@@ -682,18 +682,6 @@
   </si>
   <si>
     <t>ClassificationThreshold</t>
-  </si>
-  <si>
-    <t>DUActionCatalog</t>
-  </si>
-  <si>
-    <t>DU Insights</t>
-  </si>
-  <si>
-    <t>DUStorageBucket</t>
-  </si>
-  <si>
-    <t>DUQueue</t>
   </si>
   <si>
     <t>Classification threshold for Classification Business Rule Validation must be a value between 0 and 1.</t>
@@ -1100,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1345,7 +1333,7 @@
         <v>0.5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1353,9 +1341,7 @@
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>216</v>
-      </c>
+      <c r="B24" s="3"/>
       <c r="C24" t="s">
         <v>209</v>
       </c>
@@ -1364,9 +1350,6 @@
       <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B25" t="s">
-        <v>217</v>
-      </c>
       <c r="C25" t="s">
         <v>210</v>
       </c>
@@ -1375,9 +1358,7 @@
       <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>218</v>
-      </c>
+      <c r="B26" s="3"/>
       <c r="C26" t="s">
         <v>211</v>
       </c>
@@ -1386,9 +1367,6 @@
       <c r="A27" t="s">
         <v>119</v>
       </c>
-      <c r="B27" t="s">
-        <v>217</v>
-      </c>
       <c r="C27" t="s">
         <v>212</v>
       </c>
@@ -1397,9 +1375,7 @@
       <c r="A28" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>219</v>
-      </c>
+      <c r="B28" s="3"/>
       <c r="C28" t="s">
         <v>213</v>
       </c>
@@ -1407,9 +1383,6 @@
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>79</v>
-      </c>
-      <c r="B29" t="s">
-        <v>217</v>
       </c>
       <c r="C29" t="s">
         <v>214</v>
@@ -3844,8 +3817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3900,9 +3873,6 @@
       <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
-        <v>217</v>
-      </c>
       <c r="D2" t="s">
         <v>38</v>
       </c>
@@ -3914,9 +3884,6 @@
       <c r="B3" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C3" t="s">
-        <v>217</v>
-      </c>
       <c r="D3" s="3" t="s">
         <v>185</v>
       </c>
@@ -3928,9 +3895,6 @@
       <c r="B4" t="s">
         <v>174</v>
       </c>
-      <c r="C4" t="s">
-        <v>217</v>
-      </c>
       <c r="D4" s="3" t="s">
         <v>186</v>
       </c>
@@ -3942,9 +3906,6 @@
       <c r="B5" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C5" t="s">
-        <v>217</v>
-      </c>
       <c r="D5" s="3" t="s">
         <v>191</v>
       </c>
@@ -3955,9 +3916,6 @@
       </c>
       <c r="B6" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="C6" t="s">
-        <v>217</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>192</v>
@@ -3975,9 +3933,6 @@
       <c r="B8" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C8" t="s">
-        <v>217</v>
-      </c>
       <c r="D8" t="s">
         <v>203</v>
       </c>
@@ -3989,9 +3944,6 @@
       <c r="B9" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C9" t="s">
-        <v>217</v>
-      </c>
       <c r="D9" t="s">
         <v>204</v>
       </c>
@@ -4003,9 +3955,6 @@
       <c r="B10" t="s">
         <v>197</v>
       </c>
-      <c r="C10" t="s">
-        <v>217</v>
-      </c>
       <c r="D10" t="s">
         <v>205</v>
       </c>
@@ -4017,9 +3966,6 @@
       <c r="B11" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C11" t="s">
-        <v>217</v>
-      </c>
       <c r="D11" t="s">
         <v>206</v>
       </c>
@@ -4031,9 +3977,6 @@
       <c r="B12" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C12" t="s">
-        <v>217</v>
-      </c>
       <c r="D12" t="s">
         <v>207</v>
       </c>
@@ -4045,9 +3988,6 @@
       <c r="B13" t="s">
         <v>202</v>
       </c>
-      <c r="C13" t="s">
-        <v>217</v>
-      </c>
       <c r="D13" t="s">
         <v>208</v>
       </c>
@@ -4057,13 +3997,10 @@
         <v>215</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C14" t="s">
         <v>217</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add ReceiptPostProcessing.xaml Added 6 test cases
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandru.hojda\PycharmProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67142BE-2F6A-477E-889E-BC3A3295E6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB031118-D0A0-4A5D-AFB4-031DC7B2D195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -5063,8 +5063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5225,7 +5225,7 @@
         <v>163</v>
       </c>
       <c r="B21">
-        <v>85</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -5233,7 +5233,7 @@
         <v>164</v>
       </c>
       <c r="B22">
-        <v>80</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -5241,7 +5241,7 @@
         <v>165</v>
       </c>
       <c r="B23">
-        <v>85</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -5249,7 +5249,7 @@
         <v>166</v>
       </c>
       <c r="B24">
-        <v>85</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -5270,7 +5270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC3E61C-21FD-4D1D-AFCD-DBE631631979}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed Config after merge with develop
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandru.hojda\PycharmProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB031118-D0A0-4A5D-AFB4-031DC7B2D195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE677619-88AB-4D2E-8335-2BF57DB505FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="241">
   <si>
     <t>Name</t>
   </si>
@@ -749,6 +749,15 @@
   </si>
   <si>
     <t>Shared</t>
+  </si>
+  <si>
+    <t>ClassificationThreshold</t>
+  </si>
+  <si>
+    <t>Classification threshold for Classification Business Rule Validation must be a value between 0 and 1.</t>
+  </si>
+  <si>
+    <t>DU_ClassificationThreshold</t>
   </si>
 </sst>
 </file>
@@ -820,7 +829,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -832,6 +841,10 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1147,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1381,64 +1394,78 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="3"/>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" t="s">
-        <v>210</v>
-      </c>
-    </row>
+      <c r="A22" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>37</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B24" s="3"/>
       <c r="C24" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>36</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="3"/>
+        <v>37</v>
+      </c>
       <c r="C26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>79</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="3"/>
+    </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2411,6 +2438,8 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" xr:uid="{EF98B574-7169-43E5-821B-D4670F472688}"/>
@@ -3863,8 +3892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4065,7 +4094,41 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+    </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5063,7 +5126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added VB and C# GetTransactionItem and GetTransactionItemTestCase
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura.olaru\Desktop\GIT\DU\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB760162-D958-4309-8A46-E82C7FAB0BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A421BF9-324A-4627-8FB8-C4A9C0F1769D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3817,8 +3817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Feature/du/add try catch specific content (#197)
* Added try catch

* Added BRexception

* Added BRexception

* Started test case

* Improved testcase

* Added first version of the test case

* Added VB and C# GetTransactionItem and GetTransactionItemTestCase
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura.olaru\Desktop\GIT\DU\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB760162-D958-4309-8A46-E82C7FAB0BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A421BF9-324A-4627-8FB8-C4A9C0F1769D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3817,8 +3817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix for GetTransactionItem & associated tests
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952A7288-739C-458F-9CE9-AB325396CB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115BF191-F225-4565-A14A-2ED644F7DF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="-93" windowWidth="24693" windowHeight="14586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46908" yWindow="-108" windowWidth="30000" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="246">
   <si>
     <t>Name</t>
   </si>
@@ -770,6 +770,9 @@
   </si>
   <si>
     <t>Key in the Transaction Item's dictionary that holds the path to the file to be processed</t>
+  </si>
+  <si>
+    <t>DU_InputQueue</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1174,7 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1473,7 +1476,9 @@
       <c r="A30" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="C30" t="s">
         <v>211</v>
       </c>

</xml_diff>

<commit_message>
- Re-written 50_Extract + replaced IFE with FE, removed unnecessary sequence, updated Config.xlsx, fixed view of Mains
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\GitProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C67DC33-F5B0-4A44-A6C7-2F8AC74C5D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413E7619-D668-4E69-8645-8A9EDA2CF9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -301,12 +301,6 @@
     <t>https://du.uipath.com/svc/intelligentkeywords</t>
   </si>
   <si>
-    <t>IntelligentFormExtractorEndpoint</t>
-  </si>
-  <si>
-    <t>https://du.uipath.com/svc/intelligentforms</t>
-  </si>
-  <si>
     <t>UiPath public endpoint for classification</t>
   </si>
   <si>
@@ -776,6 +770,12 @@
   </si>
   <si>
     <t>Updating transaction progress to:</t>
+  </si>
+  <si>
+    <t>https://du.uipath.com/svc/formextractor</t>
+  </si>
+  <si>
+    <t>FormExtractorEndpoint</t>
   </si>
   <si>
     <t>DU_InputQueue</t>
@@ -853,7 +853,6 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -862,6 +861,7 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1255,13 +1255,13 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1314,7 +1314,7 @@
       <c r="A10" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>43</v>
       </c>
       <c r="C10" t="s">
@@ -1325,132 +1325,132 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>125</v>
+      <c r="B12" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
         <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" t="s">
+        <v>246</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14" t="s">
         <v>89</v>
-      </c>
-      <c r="C14" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="A17" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="C18" s="3" t="s">
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="3"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B22">
         <v>0.5</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>214</v>
+      <c r="C22" s="2" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="3"/>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>240</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C24" t="s">
         <v>242</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C24" t="s">
-        <v>244</v>
-      </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
+      <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="2"/>
       <c r="C26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1458,35 +1458,35 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="2"/>
       <c r="C28" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C29" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>247</v>
       </c>
       <c r="C30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2472,13 +2472,8 @@
     <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{EF98B574-7169-43E5-821B-D4670F472688}"/>
-    <hyperlink ref="B10" r:id="rId2" xr:uid="{A81C761C-FDC0-4FAC-9731-C4ED96819803}"/>
-    <hyperlink ref="B12" r:id="rId3" xr:uid="{25977FD7-D683-43E1-B69A-0E1CBCB81805}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2579,13 +2574,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B7">
         <v>30</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>120</v>
+      <c r="C7" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2595,8 +2590,8 @@
       <c r="B8">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>118</v>
+      <c r="C8" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2645,8 +2640,8 @@
       <c r="A16" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>96</v>
+      <c r="B16" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2661,8 +2656,8 @@
       <c r="A18" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>177</v>
+      <c r="B18" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2678,7 +2673,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2686,7 +2681,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2702,7 +2697,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2715,10 +2710,10 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2738,11 +2733,11 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>176</v>
+      <c r="B28" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2758,7 +2753,7 @@
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2774,7 +2769,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2802,135 +2797,135 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B40" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B47" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B48" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B52" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2939,7 +2934,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2964,11 +2959,11 @@
         <v>31</v>
       </c>
       <c r="B61" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
+      <c r="B62" s="3"/>
     </row>
     <row r="63" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3999,74 +3994,74 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>183</v>
+      <c r="A3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>184</v>
+        <v>170</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>189</v>
+      <c r="A5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>190</v>
+      <c r="A6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>198</v>
+      <c r="B8" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>197</v>
+      <c r="B9" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="D9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4074,32 +4069,32 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>196</v>
+        <v>115</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="D11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>199</v>
+      <c r="B12" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="D12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4107,21 +4102,21 @@
         <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>214</v>
+      <c r="D14" s="2" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5133,178 +5128,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>146</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>158</v>
+        <v>144</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>157</v>
+        <v>146</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>150</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>160</v>
+        <v>148</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="C17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>152</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>159</v>
+        <v>150</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>154</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>165</v>
+        <v>152</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="C19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>161</v>
+      <c r="A21" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="B21">
         <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>162</v>
+      <c r="A22" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="B22">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>163</v>
+      <c r="A23" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="B23">
         <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>164</v>
+      <c r="A24" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="B24">
         <v>85</v>
@@ -5312,7 +5307,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B25">
         <v>50</v>
@@ -5353,118 +5348,118 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B18">
         <v>50</v>
@@ -5472,7 +5467,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B19">
         <v>85</v>
@@ -5480,7 +5475,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B20">
         <v>50</v>

</xml_diff>

<commit_message>
*Changed other-Confidence field in IPP config sheet from 50 to 45 *Changed OutputMessageFormat in Invoice_OtherFieldsConfidence test to add more info about confidence score of the extracted fields
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/anghellos_paraskeviotis_uipath_com/Documents/Documents/_work/_projects/_uipath/Others/StudioTemplaters/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandru.hojda\Desktop\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{D622206F-3E59-4817-B3E2-F6E0C71BC575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0A0FA8B-8DC6-476A-BC0D-59696AC0524B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69551D81-9AD1-4814-A9D6-0DCD85007103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32505" yWindow="1410" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -941,10 +941,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4016,7 +4012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -5239,8 +5235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5433,7 +5429,7 @@
         <v>153</v>
       </c>
       <c r="B25">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pytests corrections and package updates
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/sergiu_wittenberger_uipath_com/Documents/PycharmProjects/StudioTemplates/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\add_pytest_v2\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69551D81-9AD1-4814-A9D6-0DCD85007103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F504FCA2-91DA-42F1-9B41-A7F1B4E54EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17892" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="272">
   <si>
     <t>Name</t>
   </si>
@@ -843,6 +843,15 @@
   </si>
   <si>
     <t>OCR Autocorrection finished</t>
+  </si>
+  <si>
+    <t>MaxExecutionAttemptsHigh</t>
+  </si>
+  <si>
+    <t>Maximum number of execution attempts for a process step which by default is high.</t>
+  </si>
+  <si>
+    <t>RetryIntervalLow</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1252,7 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2542,10 +2551,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1021"/>
+  <dimension ref="A1:Z1023"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2637,429 +2646,449 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>269</v>
       </c>
       <c r="B7">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>117</v>
+        <v>99999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="B8">
         <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>93</v>
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>174</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>170</v>
+        <v>76</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>173</v>
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>171</v>
+      <c r="A30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>265</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>266</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>267</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>268</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>265</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>267</v>
+      </c>
+      <c r="B37" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>30</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>118</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B42" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" t="s">
-        <v>96</v>
-      </c>
-    </row>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B48" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>235</v>
-      </c>
-      <c r="B49" t="s">
-        <v>236</v>
-      </c>
-    </row>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>237</v>
+        <v>112</v>
       </c>
       <c r="B50" t="s">
-        <v>238</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>235</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>237</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>242</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+    </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>242</v>
+      </c>
+      <c r="B56" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>99</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>20</v>
-      </c>
-      <c r="B62" t="s">
-        <v>17</v>
-      </c>
-    </row>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>31</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B65" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4001,6 +4030,8 @@
     <row r="1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1020" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1021" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1022" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1023" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Pytest] Take changes from PR #223 (#272)
* Changes from PR #223 [Pytest]

* Pytests corrections and package updates

* fixed the test. It seems the extraction adds a blank space between the number and the -preview line.

* cliVersion changed in DU-Test.yml

---------

Co-authored-by: Sergiu Wittenberger <sergiu.wittenberger@uipath.com>
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/sergiu_wittenberger_uipath_com/Documents/PycharmProjects/StudioTemplates/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\add_pytest_v2\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69551D81-9AD1-4814-A9D6-0DCD85007103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F504FCA2-91DA-42F1-9B41-A7F1B4E54EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17892" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="272">
   <si>
     <t>Name</t>
   </si>
@@ -843,6 +843,15 @@
   </si>
   <si>
     <t>OCR Autocorrection finished</t>
+  </si>
+  <si>
+    <t>MaxExecutionAttemptsHigh</t>
+  </si>
+  <si>
+    <t>Maximum number of execution attempts for a process step which by default is high.</t>
+  </si>
+  <si>
+    <t>RetryIntervalLow</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1252,7 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2542,10 +2551,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1021"/>
+  <dimension ref="A1:Z1023"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2637,429 +2646,449 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>269</v>
       </c>
       <c r="B7">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>117</v>
+        <v>99999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="B8">
         <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>93</v>
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>174</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>170</v>
+        <v>76</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>173</v>
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>171</v>
+      <c r="A30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>265</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>266</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>267</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>268</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>265</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>267</v>
+      </c>
+      <c r="B37" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>30</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>118</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B42" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" t="s">
-        <v>96</v>
-      </c>
-    </row>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B48" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>235</v>
-      </c>
-      <c r="B49" t="s">
-        <v>236</v>
-      </c>
-    </row>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>237</v>
+        <v>112</v>
       </c>
       <c r="B50" t="s">
-        <v>238</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>235</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>237</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>242</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+    </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>242</v>
+      </c>
+      <c r="B56" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>99</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>20</v>
-      </c>
-      <c r="B62" t="s">
-        <v>17</v>
-      </c>
-    </row>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>31</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B65" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4001,6 +4030,8 @@
     <row r="1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1020" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1021" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1022" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1023" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Pytest] Take changes from PR #223 (#272) (#273)
* Changes from PR #223 [Pytest]

* Pytests corrections and package updates

* fixed the test. It seems the extraction adds a blank space between the number and the -preview line.

* cliVersion changed in DU-Test.yml

---------

Co-authored-by: TeodoraPatrascu <104830515+TeodoraPatrascu@users.noreply.github.com>
Co-authored-by: Sergiu Wittenberger <sergiu.wittenberger@uipath.com>
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/sergiu_wittenberger_uipath_com/Documents/PycharmProjects/StudioTemplates/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\add_pytest_v2\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69551D81-9AD1-4814-A9D6-0DCD85007103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F504FCA2-91DA-42F1-9B41-A7F1B4E54EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17892" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="272">
   <si>
     <t>Name</t>
   </si>
@@ -843,6 +843,15 @@
   </si>
   <si>
     <t>OCR Autocorrection finished</t>
+  </si>
+  <si>
+    <t>MaxExecutionAttemptsHigh</t>
+  </si>
+  <si>
+    <t>Maximum number of execution attempts for a process step which by default is high.</t>
+  </si>
+  <si>
+    <t>RetryIntervalLow</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1252,7 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2542,10 +2551,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1021"/>
+  <dimension ref="A1:Z1023"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2637,429 +2646,449 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>269</v>
       </c>
       <c r="B7">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>117</v>
+        <v>99999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="B8">
         <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>93</v>
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>174</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>170</v>
+        <v>76</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>173</v>
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>171</v>
+      <c r="A30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>265</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>266</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>267</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>268</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>265</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>267</v>
+      </c>
+      <c r="B37" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>30</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>118</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B42" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" t="s">
-        <v>96</v>
-      </c>
-    </row>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B48" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>235</v>
-      </c>
-      <c r="B49" t="s">
-        <v>236</v>
-      </c>
-    </row>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>237</v>
+        <v>112</v>
       </c>
       <c r="B50" t="s">
-        <v>238</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>235</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>237</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>242</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+    </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>242</v>
+      </c>
+      <c r="B56" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>99</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>20</v>
-      </c>
-      <c r="B62" t="s">
-        <v>17</v>
-      </c>
-    </row>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>31</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B65" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4001,6 +4030,8 @@
     <row r="1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1020" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1021" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1022" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1023" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update User Guide, Config file and test input data
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\add_pytest_v2\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\Develop\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F504FCA2-91DA-42F1-9B41-A7F1B4E54EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB1BB14-885B-4DBE-9697-D6F9D66CFC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17892" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -524,9 +524,6 @@
     <t>PO Number-Confidence</t>
   </si>
   <si>
-    <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms, Currency,Discount</t>
-  </si>
-  <si>
     <t>True</t>
   </si>
   <si>
@@ -852,6 +849,9 @@
   </si>
   <si>
     <t>RetryIntervalLow</t>
+  </si>
+  <si>
+    <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms,Discount</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1333,7 @@
         <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1428,59 +1428,59 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>179</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1490,13 +1490,13 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B22">
         <v>0.5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1504,13 +1504,13 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>238</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" t="s">
         <v>240</v>
-      </c>
-      <c r="C24" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1522,7 +1522,7 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1530,7 +1530,7 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1547,7 +1547,7 @@
         <v>114</v>
       </c>
       <c r="C29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1555,10 +1555,10 @@
         <v>78</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1566,7 +1566,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2553,8 +2553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2646,13 +2646,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B7">
         <v>99999</v>
       </c>
       <c r="C7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2679,7 +2679,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2751,7 +2751,7 @@
         <v>76</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2767,7 +2767,7 @@
         <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2775,7 +2775,7 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2791,7 +2791,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2831,7 +2831,7 @@
         <v>77</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2847,7 +2847,7 @@
         <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2863,7 +2863,7 @@
         <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2876,18 +2876,18 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>264</v>
+      </c>
+      <c r="B36" t="s">
         <v>265</v>
-      </c>
-      <c r="B36" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>266</v>
+      </c>
+      <c r="B37" t="s">
         <v>267</v>
-      </c>
-      <c r="B37" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2908,18 +2908,18 @@
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2975,18 +2975,18 @@
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>234</v>
+      </c>
+      <c r="B51" t="s">
         <v>235</v>
-      </c>
-      <c r="B51" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>236</v>
+      </c>
+      <c r="B52" t="s">
         <v>237</v>
-      </c>
-      <c r="B52" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3015,10 +3015,10 @@
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>241</v>
+      </c>
+      <c r="B56" t="s">
         <v>242</v>
-      </c>
-      <c r="B56" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3035,7 +3035,7 @@
         <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3044,7 +3044,7 @@
         <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3069,7 +3069,7 @@
         <v>31</v>
       </c>
       <c r="B65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4105,46 +4105,46 @@
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4157,10 +4157,10 @@
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4168,10 +4168,10 @@
         <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4179,10 +4179,10 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4190,10 +4190,10 @@
         <v>114</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4201,10 +4201,10 @@
         <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4212,66 +4212,66 @@
         <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" t="s">
         <v>257</v>
-      </c>
-      <c r="D16" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" t="s">
         <v>259</v>
-      </c>
-      <c r="D17" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B18" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" t="s">
         <v>261</v>
-      </c>
-      <c r="D18" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B19" t="s">
+        <v>262</v>
+      </c>
+      <c r="D19" t="s">
         <v>263</v>
-      </c>
-      <c r="D19" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5266,8 +5266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5417,7 +5417,7 @@
         <v>151</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>162</v>
+        <v>271</v>
       </c>
       <c r="C19" t="s">
         <v>152</v>
@@ -5474,7 +5474,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5498,15 +5498,15 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" t="s">
         <v>213</v>
-      </c>
-      <c r="B3" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
         <v>126</v>
@@ -5514,7 +5514,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B5" t="s">
         <v>128</v>
@@ -5522,7 +5522,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s">
         <v>134</v>
@@ -5530,7 +5530,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -5538,15 +5538,15 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
         <v>219</v>
-      </c>
-      <c r="B8" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s">
         <v>142</v>
@@ -5554,10 +5554,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" t="s">
         <v>222</v>
-      </c>
-      <c r="B12" t="s">
-        <v>223</v>
       </c>
       <c r="C12" t="s">
         <v>144</v>
@@ -5565,10 +5565,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" t="s">
         <v>224</v>
-      </c>
-      <c r="B13" t="s">
-        <v>225</v>
       </c>
       <c r="C13" t="s">
         <v>146</v>
@@ -5576,10 +5576,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14" t="s">
         <v>226</v>
-      </c>
-      <c r="B14" t="s">
-        <v>227</v>
       </c>
       <c r="C14" t="s">
         <v>148</v>
@@ -5587,10 +5587,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" t="s">
         <v>228</v>
-      </c>
-      <c r="B15" t="s">
-        <v>229</v>
       </c>
       <c r="C15" t="s">
         <v>150</v>
@@ -5598,10 +5598,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16" t="s">
         <v>230</v>
-      </c>
-      <c r="B16" t="s">
-        <v>231</v>
       </c>
       <c r="C16" t="s">
         <v>152</v>
@@ -5609,7 +5609,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B18">
         <v>50</v>
@@ -5617,7 +5617,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B19">
         <v>85</v>
@@ -5625,7 +5625,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B20">
         <v>50</v>
@@ -5716,44 +5716,44 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" t="s">
         <v>248</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>249</v>
-      </c>
-      <c r="C3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" t="s">
         <v>255</v>
-      </c>
-      <c r="C7" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Feature/du/update template for active learning (#283)
* Update packages for Document Understanding template.

* Update User Guide, Config file and test input data

* Update Config_Expected.xlsx file, removed Currency.

* Rearrange all the flowcharts in the template

* Rearrange the flowcharts in the InvoicePostProcessing_mock_4.xaml
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\add_pytest_v2\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\Develop\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F504FCA2-91DA-42F1-9B41-A7F1B4E54EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB1BB14-885B-4DBE-9697-D6F9D66CFC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17892" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -524,9 +524,6 @@
     <t>PO Number-Confidence</t>
   </si>
   <si>
-    <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms, Currency,Discount</t>
-  </si>
-  <si>
     <t>True</t>
   </si>
   <si>
@@ -852,6 +849,9 @@
   </si>
   <si>
     <t>RetryIntervalLow</t>
+  </si>
+  <si>
+    <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms,Discount</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1333,7 @@
         <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1428,59 +1428,59 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>179</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1490,13 +1490,13 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B22">
         <v>0.5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1504,13 +1504,13 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>238</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" t="s">
         <v>240</v>
-      </c>
-      <c r="C24" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1522,7 +1522,7 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1530,7 +1530,7 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1547,7 +1547,7 @@
         <v>114</v>
       </c>
       <c r="C29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1555,10 +1555,10 @@
         <v>78</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1566,7 +1566,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2553,8 +2553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2646,13 +2646,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B7">
         <v>99999</v>
       </c>
       <c r="C7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2679,7 +2679,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2751,7 +2751,7 @@
         <v>76</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2767,7 +2767,7 @@
         <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2775,7 +2775,7 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2791,7 +2791,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2831,7 +2831,7 @@
         <v>77</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2847,7 +2847,7 @@
         <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2863,7 +2863,7 @@
         <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2876,18 +2876,18 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>264</v>
+      </c>
+      <c r="B36" t="s">
         <v>265</v>
-      </c>
-      <c r="B36" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>266</v>
+      </c>
+      <c r="B37" t="s">
         <v>267</v>
-      </c>
-      <c r="B37" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2908,18 +2908,18 @@
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2975,18 +2975,18 @@
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>234</v>
+      </c>
+      <c r="B51" t="s">
         <v>235</v>
-      </c>
-      <c r="B51" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>236</v>
+      </c>
+      <c r="B52" t="s">
         <v>237</v>
-      </c>
-      <c r="B52" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3015,10 +3015,10 @@
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>241</v>
+      </c>
+      <c r="B56" t="s">
         <v>242</v>
-      </c>
-      <c r="B56" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3035,7 +3035,7 @@
         <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3044,7 +3044,7 @@
         <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3069,7 +3069,7 @@
         <v>31</v>
       </c>
       <c r="B65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4105,46 +4105,46 @@
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4157,10 +4157,10 @@
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4168,10 +4168,10 @@
         <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4179,10 +4179,10 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4190,10 +4190,10 @@
         <v>114</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4201,10 +4201,10 @@
         <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4212,66 +4212,66 @@
         <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" t="s">
         <v>257</v>
-      </c>
-      <c r="D16" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" t="s">
         <v>259</v>
-      </c>
-      <c r="D17" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B18" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" t="s">
         <v>261</v>
-      </c>
-      <c r="D18" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B19" t="s">
+        <v>262</v>
+      </c>
+      <c r="D19" t="s">
         <v>263</v>
-      </c>
-      <c r="D19" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5266,8 +5266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5417,7 +5417,7 @@
         <v>151</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>162</v>
+        <v>271</v>
       </c>
       <c r="C19" t="s">
         <v>152</v>
@@ -5474,7 +5474,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5498,15 +5498,15 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" t="s">
         <v>213</v>
-      </c>
-      <c r="B3" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
         <v>126</v>
@@ -5514,7 +5514,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B5" t="s">
         <v>128</v>
@@ -5522,7 +5522,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s">
         <v>134</v>
@@ -5530,7 +5530,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -5538,15 +5538,15 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
         <v>219</v>
-      </c>
-      <c r="B8" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s">
         <v>142</v>
@@ -5554,10 +5554,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" t="s">
         <v>222</v>
-      </c>
-      <c r="B12" t="s">
-        <v>223</v>
       </c>
       <c r="C12" t="s">
         <v>144</v>
@@ -5565,10 +5565,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" t="s">
         <v>224</v>
-      </c>
-      <c r="B13" t="s">
-        <v>225</v>
       </c>
       <c r="C13" t="s">
         <v>146</v>
@@ -5576,10 +5576,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14" t="s">
         <v>226</v>
-      </c>
-      <c r="B14" t="s">
-        <v>227</v>
       </c>
       <c r="C14" t="s">
         <v>148</v>
@@ -5587,10 +5587,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" t="s">
         <v>228</v>
-      </c>
-      <c r="B15" t="s">
-        <v>229</v>
       </c>
       <c r="C15" t="s">
         <v>150</v>
@@ -5598,10 +5598,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16" t="s">
         <v>230</v>
-      </c>
-      <c r="B16" t="s">
-        <v>231</v>
       </c>
       <c r="C16" t="s">
         <v>152</v>
@@ -5609,7 +5609,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B18">
         <v>50</v>
@@ -5617,7 +5617,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B19">
         <v>85</v>
@@ -5625,7 +5625,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B20">
         <v>50</v>
@@ -5716,44 +5716,44 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" t="s">
         <v>248</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>249</v>
-      </c>
-      <c r="C3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" t="s">
         <v>255</v>
-      </c>
-      <c r="C7" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Windows VB - Rearrange the main flow horizontally;update date parse in IPP and RPP Cross-platform - Rearrange the main flow horizontally;changes to IPP and RPP to use FieldId instead of FieldName and change date parse;update config.json to use the field ids and not the fields names for invoice and receipt
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\Cross_platform\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C369CC-C0D2-4ACF-9956-E974F6E6C10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A01397E-3AAB-4F11-B26E-F3DB33EBF693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9468" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9468" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="274">
   <si>
     <t>Name</t>
   </si>
@@ -836,9 +836,6 @@
     <t>RetryIntervalLow</t>
   </si>
   <si>
-    <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms,Discount</t>
-  </si>
-  <si>
     <t>AutocorrectionLearningFile.json</t>
   </si>
   <si>
@@ -849,6 +846,18 @@
   </si>
   <si>
     <t>DU_AutocorrectionFieldIdList</t>
+  </si>
+  <si>
+    <t>DU_DateFormats</t>
+  </si>
+  <si>
+    <t>Different date formats.</t>
+  </si>
+  <si>
+    <t>yyyy-MM-dd;dd-MM-yyyy;MM-dd-yyyy;MM/dd/yyyy;dd/MM/yyyy;yyyy/MM/dd;dd.MM.yyyy;MM.dd.yyyy;yyyy.MM.dd</t>
+  </si>
+  <si>
+    <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms</t>
   </si>
 </sst>
 </file>
@@ -1246,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1006"/>
+  <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1435,138 +1444,150 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>162</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>178</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>184</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="2"/>
+      <c r="A21" t="s">
+        <v>209</v>
+      </c>
+      <c r="B21">
+        <v>0.5</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>209</v>
-      </c>
-      <c r="B22">
-        <v>0.5</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>210</v>
-      </c>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="2"/>
+      <c r="A23" t="s">
+        <v>238</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C23" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>238</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C24" t="s">
-        <v>240</v>
-      </c>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
+      <c r="A25" t="s">
+        <v>270</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C25" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>35</v>
-      </c>
       <c r="B26" s="2"/>
-      <c r="C26" t="s">
-        <v>203</v>
-      </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B27" s="2"/>
       <c r="C27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="2"/>
+        <v>36</v>
+      </c>
       <c r="C28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>114</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B29" s="2"/>
       <c r="C29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>245</v>
+        <v>114</v>
       </c>
       <c r="C30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>79</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2540,6 +2561,7 @@
     <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4040,7 +4062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -4262,13 +4284,13 @@
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>267</v>
+      </c>
+      <c r="B19" t="s">
+        <v>269</v>
+      </c>
+      <c r="D19" t="s">
         <v>268</v>
-      </c>
-      <c r="B19" t="s">
-        <v>270</v>
-      </c>
-      <c r="D19" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5263,8 +5285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5414,7 +5436,7 @@
         <v>151</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C19" t="s">
         <v>152</v>
@@ -5716,7 +5738,7 @@
         <v>247</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C3" t="s">
         <v>248</v>
@@ -5747,10 +5769,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C7" t="s">
         <v>268</v>
-      </c>
-      <c r="C7" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Windows VB - add DU_DateFormats as Asset as well Cross-platform - add DU_DateFormats as Asset as well
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\Cross_platform\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A01397E-3AAB-4F11-B26E-F3DB33EBF693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0DF345-8765-405C-AFF6-B1BB63538D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9468" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21252" yWindow="-17568" windowWidth="30936" windowHeight="17040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="274">
   <si>
     <t>Name</t>
   </si>
@@ -1257,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="B5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4062,8 +4062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4294,7 +4294,17 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>270</v>
+      </c>
+      <c r="B21" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" t="s">
+        <v>271</v>
+      </c>
+    </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5285,7 +5295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>